<commit_message>
Added a Project Milestones Document
Added a Project Milestones.xlsx document to help keep track of the sprint requirements.
</commit_message>
<xml_diff>
--- a/docs/Project Milestones.xlsx
+++ b/docs/Project Milestones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nictus/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nictus/Dev/repos/designpatternsfinalprivatef23-galactic/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AC0117-1120-D040-B544-6F90F1523621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D770A779-BA5C-D647-9A0E-38DFB3E01E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{D9D828B8-6435-C545-8999-EDE37590929C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Pattern</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Board and board factory. Board factory takes dimensions for a map as a grid and selects starting locations for the units. Returns the Board object which contains the units and tiles.</t>
   </si>
   <si>
-    <t>All units are moveable and implement Moveable, which has a .move() method.</t>
-  </si>
-  <si>
     <t>Implementation/Design Notes</t>
   </si>
   <si>
@@ -96,6 +93,21 @@
   </si>
   <si>
     <t>Control of the R/W access to the file that will hard-coded sheet of the creature features</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>An interface ProgressibleUnit that has a method called progress() to handle everything each unit needs to do with each game iterration.</t>
+  </si>
+  <si>
+    <t>Vince</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Rocky</t>
   </si>
 </sst>
 </file>
@@ -462,7 +474,7 @@
       <pane xSplit="5" ySplit="19" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,24 +499,30 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -516,11 +534,14 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -538,33 +559,42 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>